<commit_message>
iftar and sehri time test
</commit_message>
<xml_diff>
--- a/2025/table.xlsx
+++ b/2025/table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2244c9b051158813/Documents/git-repo/iftar-countdown/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC10485DE9DB43C45BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39D573B0-98D4-456B-AFF7-EF44182AE4A5}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10485DE9DB43C45BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56CC6CD7-8B3E-45E0-AA41-D6A6C28663D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>তারখি</t>
   </si>
@@ -124,6 +125,9 @@
   </si>
   <si>
     <t>৩১ র্মাচ</t>
+  </si>
+  <si>
+    <t>০১ এপ্রিল</t>
   </si>
 </sst>
 </file>
@@ -133,13 +137,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-5000000]h:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Noto Sans Bengali"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,9 +171,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,348 +468,372 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.25138888888888888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.25208333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.25208333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
         <v>0.20902777777777778</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C5" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.2076388888888889</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.20902777777777778</v>
-      </c>
-      <c r="C3" s="1">
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.20694444444444443</v>
+      </c>
+      <c r="C8" s="2">
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.20902777777777778</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.25347222222222221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.20902777777777778</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.25347222222222221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
         <v>0.20624999999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C9" s="2">
+        <v>0.25416666666666665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.20555555555555555</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.25416666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.25416666666666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.20416666666666666</v>
+      </c>
+      <c r="C12" s="2">
         <v>0.25486111111111109</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.20624999999999999</v>
-      </c>
-      <c r="C7" s="1">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.20347222222222222</v>
+      </c>
+      <c r="C13" s="2">
         <v>0.25486111111111109</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.20624999999999999</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.20624999999999999</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.20624999999999999</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.20624999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
+    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.20277777777777778</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.25555555555555554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
         <v>0.20208333333333334</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="2">
+        <v>0.25555555555555554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.25555555555555554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.20069444444444445</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.25624999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.25624999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.19930555555555557</v>
+      </c>
+      <c r="C19" s="2">
         <v>0.25694444444444442</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.2013888888888889</v>
-      </c>
-      <c r="C13" s="1">
+    <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.1986111111111111</v>
+      </c>
+      <c r="C20" s="2">
         <v>0.25694444444444442</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.20069444444444445</v>
-      </c>
-      <c r="C14" s="1">
+    <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.25694444444444442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.19722222222222222</v>
+      </c>
+      <c r="C22" s="2">
         <v>0.25763888888888886</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C15" s="1">
+    <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="C23" s="2">
         <v>0.25763888888888886</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.19930555555555557</v>
-      </c>
-      <c r="C16" s="1">
+    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.19583333333333333</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.25763888888888886</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.19513888888888889</v>
+      </c>
+      <c r="C25" s="2">
         <v>0.25833333333333336</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.1986111111111111</v>
-      </c>
-      <c r="C17" s="1">
+    <row r="26" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="C26" s="2">
         <v>0.25833333333333336</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.19791666666666666</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.25833333333333336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.19722222222222222</v>
-      </c>
-      <c r="C19" s="1">
+    <row r="27" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.19375000000000001</v>
+      </c>
+      <c r="C27" s="2">
         <v>0.2590277777777778</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.19652777777777777</v>
-      </c>
-      <c r="C20" s="1">
+    <row r="28" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.19305555555555556</v>
+      </c>
+      <c r="C28" s="2">
         <v>0.2590277777777778</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.19583333333333333</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.2590277777777778</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.19513888888888889</v>
-      </c>
-      <c r="C22" s="1">
+    <row r="29" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.19166666666666668</v>
+      </c>
+      <c r="C29" s="2">
         <v>0.25972222222222224</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="C23" s="1">
+    <row r="30" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.19097222222222221</v>
+      </c>
+      <c r="C30" s="2">
         <v>0.25972222222222224</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.19375000000000001</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.25972222222222224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.19305555555555556</v>
-      </c>
-      <c r="C25" s="1">
+    <row r="31" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="C31" s="2">
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.19166666666666668</v>
-      </c>
-      <c r="C26" s="1">
+    <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="C32" s="2">
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.19097222222222221</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.26111111111111113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.19027777777777777</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.26111111111111113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.18958333333333333</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.26180555555555557</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0.18819444444444444</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.26180555555555557</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.1875</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.26250000000000001</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AE4686-A6C8-4CF9-BAD4-55893186EC02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>